<commit_message>
Updated battery and power sheet
</commit_message>
<xml_diff>
--- a/Documentation/Power_Excel.xlsx
+++ b/Documentation/Power_Excel.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Heddle\OneDrive\Desktop\AI-Robot\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heddl\OneDrive\Desktop\AI-Robot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C7C2E45-179D-4B06-B81F-28A457A4C5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A6892B-9C53-4976-8674-0C605066329B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50FC77DF-9D76-4291-B9A3-555CAC01C5B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{50FC77DF-9D76-4291-B9A3-555CAC01C5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="RDS5160_Servo">Sheet1!$A$2:$A$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Component</t>
   </si>
@@ -53,42 +56,15 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>14 ~ 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6V </t>
-  </si>
-  <si>
     <t>7.4V</t>
   </si>
   <si>
-    <t>8V</t>
-  </si>
-  <si>
-    <t>4 mA</t>
-  </si>
-  <si>
-    <t>5 mA</t>
-  </si>
-  <si>
-    <t>6 mA</t>
-  </si>
-  <si>
-    <t>3.5 A</t>
-  </si>
-  <si>
-    <t>6.2 A</t>
-  </si>
-  <si>
     <t>5 A</t>
   </si>
   <si>
     <t>RDS5160 Servo</t>
   </si>
   <si>
-    <t>Jetson Orin Nano (15W Mode)</t>
-  </si>
-  <si>
     <t>Jetson Orin Nano (25W Mode)</t>
   </si>
   <si>
@@ -98,18 +74,12 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>1.01~1.25 A</t>
-  </si>
-  <si>
     <t>1.69~2.08 A</t>
   </si>
   <si>
     <t>Battery Specs</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>5V</t>
   </si>
   <si>
@@ -123,6 +93,36 @@
   </si>
   <si>
     <t>170~180 mA</t>
+  </si>
+  <si>
+    <t>Running Current</t>
+  </si>
+  <si>
+    <t>5-10 mA</t>
+  </si>
+  <si>
+    <t>120-160 mA</t>
+  </si>
+  <si>
+    <t>1.2-2.0 A</t>
+  </si>
+  <si>
+    <t>500 mA</t>
+  </si>
+  <si>
+    <t>60 mA</t>
+  </si>
+  <si>
+    <t>DS3218MG MS24 Servo</t>
+  </si>
+  <si>
+    <t>14.8V</t>
+  </si>
+  <si>
+    <t>4000mAh</t>
+  </si>
+  <si>
+    <t>240A Max Draw</t>
   </si>
 </sst>
 </file>
@@ -224,26 +224,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}" name="Table2" displayName="Table2" ref="A1:E11" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Title">
-  <autoFilter ref="A1:E11" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35F05902-41A9-4FE1-8CD1-4E173F308287}" name="Table3" displayName="Table3" ref="I1:I9" totalsRowShown="0" headerRowCellStyle="Title">
+  <autoFilter ref="I1:I9" xr:uid="{35F05902-41A9-4FE1-8CD1-4E173F308287}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{D3506CEC-6495-4E6E-BD36-21F11D7C50F1}" name="Battery Specs"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}" name="Table2" displayName="Table2" ref="A1:F12" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Output">
+  <autoFilter ref="A1:F12" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E0A8BA42-5823-454F-A863-FF3C094B4D93}" name="Component"/>
     <tableColumn id="2" xr3:uid="{C44E7B69-826C-4A7E-AB63-A6C3D96DDB39}" name="Idle Current"/>
+    <tableColumn id="5" xr3:uid="{1962EF49-B829-469A-8782-6E167F3203C3}" name="Running Current"/>
     <tableColumn id="3" xr3:uid="{86F92FE7-D8FD-488A-AAC0-BF15C3F73EEF}" name="Stall Current"/>
     <tableColumn id="4" xr3:uid="{EFE6857A-BF53-486E-8762-011E151900CE}" name="Voltage"/>
     <tableColumn id="6" xr3:uid="{B89D11CA-A883-4EA4-97F0-A75FE2CDEDD6}" name="Quantity"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35F05902-41A9-4FE1-8CD1-4E173F308287}" name="Table3" displayName="Table3" ref="H1:H9" totalsRowShown="0" headerRowCellStyle="Title">
-  <autoFilter ref="H1:H9" xr:uid="{35F05902-41A9-4FE1-8CD1-4E173F308287}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D3506CEC-6495-4E6E-BD36-21F11D7C50F1}" name="Battery Specs"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -564,26 +565,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D132DD-E8ED-476D-A89F-857413B9F2C3}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="11" width="19.28515625" customWidth="1"/>
+    <col min="10" max="11" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,139 +593,136 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="5">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>5</v>
+      <c r="F6" s="5">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed to new battery
</commit_message>
<xml_diff>
--- a/Documentation/Power_Excel.xlsx
+++ b/Documentation/Power_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heddl\OneDrive\Desktop\AI-Robot\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Heddle\OneDrive\Desktop\AI-Robot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A6892B-9C53-4976-8674-0C605066329B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E0A840-A570-4921-9133-124AAA076B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{50FC77DF-9D76-4291-B9A3-555CAC01C5B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50FC77DF-9D76-4291-B9A3-555CAC01C5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,10 +119,10 @@
     <t>14.8V</t>
   </si>
   <si>
-    <t>4000mAh</t>
-  </si>
-  <si>
-    <t>240A Max Draw</t>
+    <t>5000mAh</t>
+  </si>
+  <si>
+    <t>500A Max Draw</t>
   </si>
 </sst>
 </file>
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}" name="Table2" displayName="Table2" ref="A1:F12" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}" name="Table2" displayName="Table2" ref="A1:F12" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:F12" xr:uid="{69C44DDA-9B13-4C46-BD29-367500B44AFB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E0A8BA42-5823-454F-A863-FF3C094B4D93}" name="Component"/>
@@ -568,24 +568,24 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="11" width="19.33203125" customWidth="1"/>
+    <col min="10" max="11" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -611,7 +611,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -634,7 +634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -657,7 +657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -680,7 +680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -720,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>

</xml_diff>